<commit_message>
added decription_codes_new file for self
</commit_message>
<xml_diff>
--- a/outputs/Diagnosis/description_codes_new.xlsx
+++ b/outputs/Diagnosis/description_codes_new.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="icd9" sheetId="2" r:id="rId3"/>
     <sheet name="icd10" sheetId="3" r:id="rId5"/>
+    <sheet name="self" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6180" uniqueCount="3866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6387" uniqueCount="4036">
   <si>
     <t>labels_new_icd9</t>
   </si>
@@ -11613,6 +11614,516 @@
   </si>
   <si>
     <t>K297</t>
+  </si>
+  <si>
+    <t>labels_new_self</t>
+  </si>
+  <si>
+    <t>Ischaemic heart disease</t>
+  </si>
+  <si>
+    <t>Hypertensive diseases</t>
+  </si>
+  <si>
+    <t>Stroke</t>
+  </si>
+  <si>
+    <t>COPD</t>
+  </si>
+  <si>
+    <t>CKD</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Cirrhosis</t>
+  </si>
+  <si>
+    <t>Osteoarthritis</t>
+  </si>
+  <si>
+    <t>Osteoporosis</t>
+  </si>
+  <si>
+    <t>Dementia</t>
+  </si>
+  <si>
+    <t>Parkinsonism</t>
+  </si>
+  <si>
+    <t>Multiple sclerosis</t>
+  </si>
+  <si>
+    <t>Schizophrenia</t>
+  </si>
+  <si>
+    <t>Depression</t>
+  </si>
+  <si>
+    <t>Bipolar</t>
+  </si>
+  <si>
+    <t>Anemia</t>
+  </si>
+  <si>
+    <t>Crohn disease</t>
+  </si>
+  <si>
+    <t>Ulcerative colitis</t>
+  </si>
+  <si>
+    <t>Epilepsy</t>
+  </si>
+  <si>
+    <t>Migraine</t>
+  </si>
+  <si>
+    <t>Sleep apnoea</t>
+  </si>
+  <si>
+    <t>Anorexia nervosa</t>
+  </si>
+  <si>
+    <t>Anxiety or GAD (not inc. social anxiety)</t>
+  </si>
+  <si>
+    <t>Bulimia nervosa</t>
+  </si>
+  <si>
+    <t>OCD</t>
+  </si>
+  <si>
+    <t>Panic attacks</t>
+  </si>
+  <si>
+    <t>Rheumatoid arthritis</t>
+  </si>
+  <si>
+    <t>Glomerular diseases</t>
+  </si>
+  <si>
+    <t>Renal failure</t>
+  </si>
+  <si>
+    <t>Hepatitis</t>
+  </si>
+  <si>
+    <t>Asthma</t>
+  </si>
+  <si>
+    <t>Emphysema</t>
+  </si>
+  <si>
+    <t>Cystic fibrosis</t>
+  </si>
+  <si>
+    <t>Gastro-oesophageal reflux disease (GORD)</t>
+  </si>
+  <si>
+    <t>Oesophagitis</t>
+  </si>
+  <si>
+    <t>Dermatitis and eczema</t>
+  </si>
+  <si>
+    <t>Gastritis</t>
+  </si>
+  <si>
+    <t>description_new_self</t>
+  </si>
+  <si>
+    <t>iron deficiency anaemia</t>
+  </si>
+  <si>
+    <t>pernicious anaemia</t>
+  </si>
+  <si>
+    <t>aplastic anaemia</t>
+  </si>
+  <si>
+    <t>anaemia</t>
+  </si>
+  <si>
+    <t>colitis/not crohns or ulcerative colitis</t>
+  </si>
+  <si>
+    <t>inflammatory bowel disease</t>
+  </si>
+  <si>
+    <t>crohns disease</t>
+  </si>
+  <si>
+    <t>colitis/not crohns or ulcerative colitis</t>
+  </si>
+  <si>
+    <t>inflammatory bowel disease</t>
+  </si>
+  <si>
+    <t>ulcerative colitis</t>
+  </si>
+  <si>
+    <t>dementia/alzheimers/cognitive impairment</t>
+  </si>
+  <si>
+    <t>epilepsy</t>
+  </si>
+  <si>
+    <t>migraine</t>
+  </si>
+  <si>
+    <t>headaches (not migraine)</t>
+  </si>
+  <si>
+    <t>multiple sclerosis</t>
+  </si>
+  <si>
+    <t>other demyelinating disease (not multiple sclerosis)</t>
+  </si>
+  <si>
+    <t>parkinsons disease</t>
+  </si>
+  <si>
+    <t>wolff parkinson white / wpw syndrome</t>
+  </si>
+  <si>
+    <t>sleep apnoea</t>
+  </si>
+  <si>
+    <t>anorexia/bulimia/other eating disorder</t>
+  </si>
+  <si>
+    <t>anxiety/panic attacks</t>
+  </si>
+  <si>
+    <t>mania/bipolar disorder/manic depression</t>
+  </si>
+  <si>
+    <t>iron deficiency anaemia</t>
+  </si>
+  <si>
+    <t>pernicious anaemia</t>
+  </si>
+  <si>
+    <t>aplastic anaemia</t>
+  </si>
+  <si>
+    <t>anaemia</t>
+  </si>
+  <si>
+    <t>colitis/not crohns or ulcerative colitis</t>
+  </si>
+  <si>
+    <t>inflammatory bowel disease</t>
+  </si>
+  <si>
+    <t>crohns disease</t>
+  </si>
+  <si>
+    <t>colitis/not crohns or ulcerative colitis</t>
+  </si>
+  <si>
+    <t>inflammatory bowel disease</t>
+  </si>
+  <si>
+    <t>ulcerative colitis</t>
+  </si>
+  <si>
+    <t>epilepsy</t>
+  </si>
+  <si>
+    <t>migraine</t>
+  </si>
+  <si>
+    <t>headaches (not migraine)</t>
+  </si>
+  <si>
+    <t>sleep apnoea</t>
+  </si>
+  <si>
+    <t>anorexia/bulimia/other eating disorder</t>
+  </si>
+  <si>
+    <t>anxiety/panic attacks</t>
+  </si>
+  <si>
+    <t>anorexia/bulimia/other eating disorder</t>
+  </si>
+  <si>
+    <t>obsessive compulsive disorder (ocd)</t>
+  </si>
+  <si>
+    <t>anxiety/panic attacks</t>
+  </si>
+  <si>
+    <t>rheumatoid arthritis</t>
+  </si>
+  <si>
+    <t>pyelonephritis</t>
+  </si>
+  <si>
+    <t>nephritis</t>
+  </si>
+  <si>
+    <t>glomerulnephritis</t>
+  </si>
+  <si>
+    <t>renal/kidney failure</t>
+  </si>
+  <si>
+    <t>renal failure requiring dialysis</t>
+  </si>
+  <si>
+    <t>renal failure not requiring dialysis</t>
+  </si>
+  <si>
+    <t>hepatitis</t>
+  </si>
+  <si>
+    <t>infective/viral hepatitis</t>
+  </si>
+  <si>
+    <t>non-infective hepatitis</t>
+  </si>
+  <si>
+    <t>hepatitis a</t>
+  </si>
+  <si>
+    <t>hepatitis b</t>
+  </si>
+  <si>
+    <t>hepatitis c</t>
+  </si>
+  <si>
+    <t>hepatitis d</t>
+  </si>
+  <si>
+    <t>hepatitis e</t>
+  </si>
+  <si>
+    <t>asthma</t>
+  </si>
+  <si>
+    <t>emphysema/chronic bronchitis</t>
+  </si>
+  <si>
+    <t>emphysema</t>
+  </si>
+  <si>
+    <t>fibrocystic disease</t>
+  </si>
+  <si>
+    <t>gastro-oesophageal reflux (gord) / gastric reflux</t>
+  </si>
+  <si>
+    <t>oesophagitis/barretts oesophagus</t>
+  </si>
+  <si>
+    <t>eczema/dermatitis</t>
+  </si>
+  <si>
+    <t>contact dermatitis</t>
+  </si>
+  <si>
+    <t>gastritis/gastric erosions</t>
+  </si>
+  <si>
+    <t>code_new_self</t>
+  </si>
+  <si>
+    <t>1331</t>
+  </si>
+  <si>
+    <t>1332</t>
+  </si>
+  <si>
+    <t>1339</t>
+  </si>
+  <si>
+    <t>1447</t>
+  </si>
+  <si>
+    <t>1460</t>
+  </si>
+  <si>
+    <t>1462</t>
+  </si>
+  <si>
+    <t>1463</t>
+  </si>
+  <si>
+    <t>1460</t>
+  </si>
+  <si>
+    <t>1462</t>
+  </si>
+  <si>
+    <t>1464</t>
+  </si>
+  <si>
+    <t>1264</t>
+  </si>
+  <si>
+    <t>1265</t>
+  </si>
+  <si>
+    <t>1266</t>
+  </si>
+  <si>
+    <t>1437</t>
+  </si>
+  <si>
+    <t>1262</t>
+  </si>
+  <si>
+    <t>1398</t>
+  </si>
+  <si>
+    <t>1263</t>
+  </si>
+  <si>
+    <t>1485</t>
+  </si>
+  <si>
+    <t>1124</t>
+  </si>
+  <si>
+    <t>1471</t>
+  </si>
+  <si>
+    <t>1288</t>
+  </si>
+  <si>
+    <t>1293</t>
+  </si>
+  <si>
+    <t>1331</t>
+  </si>
+  <si>
+    <t>1332</t>
+  </si>
+  <si>
+    <t>1339</t>
+  </si>
+  <si>
+    <t>1447</t>
+  </si>
+  <si>
+    <t>1460</t>
+  </si>
+  <si>
+    <t>1462</t>
+  </si>
+  <si>
+    <t>1463</t>
+  </si>
+  <si>
+    <t>1460</t>
+  </si>
+  <si>
+    <t>1462</t>
+  </si>
+  <si>
+    <t>1464</t>
+  </si>
+  <si>
+    <t>1265</t>
+  </si>
+  <si>
+    <t>1266</t>
+  </si>
+  <si>
+    <t>1437</t>
+  </si>
+  <si>
+    <t>1124</t>
+  </si>
+  <si>
+    <t>1471</t>
+  </si>
+  <si>
+    <t>1288</t>
+  </si>
+  <si>
+    <t>1471</t>
+  </si>
+  <si>
+    <t>1616</t>
+  </si>
+  <si>
+    <t>1288</t>
+  </si>
+  <si>
+    <t>1465</t>
+  </si>
+  <si>
+    <t>1516</t>
+  </si>
+  <si>
+    <t>1609</t>
+  </si>
+  <si>
+    <t>1610</t>
+  </si>
+  <si>
+    <t>1193</t>
+  </si>
+  <si>
+    <t>1194</t>
+  </si>
+  <si>
+    <t>1196</t>
+  </si>
+  <si>
+    <t>1156</t>
+  </si>
+  <si>
+    <t>1157</t>
+  </si>
+  <si>
+    <t>1158</t>
+  </si>
+  <si>
+    <t>1579</t>
+  </si>
+  <si>
+    <t>1580</t>
+  </si>
+  <si>
+    <t>1581</t>
+  </si>
+  <si>
+    <t>1582</t>
+  </si>
+  <si>
+    <t>1583</t>
+  </si>
+  <si>
+    <t>1112</t>
+  </si>
+  <si>
+    <t>1114</t>
+  </si>
+  <si>
+    <t>1473</t>
+  </si>
+  <si>
+    <t>1367</t>
+  </si>
+  <si>
+    <t>1139</t>
+  </si>
+  <si>
+    <t>1140</t>
+  </si>
+  <si>
+    <t>1453</t>
+  </si>
+  <si>
+    <t>1670</t>
+  </si>
+  <si>
+    <t>1154</t>
   </si>
 </sst>
 </file>
@@ -11633,7 +12144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -11642,15 +12153,13 @@
       <diagonal/>
     </border>
     <border/>
-    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -34344,4 +34853,807 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" customWidth="true"/>
+    <col min="2" max="2" width="47.28515625" customWidth="true"/>
+    <col min="3" max="3" width="14.5703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>3866</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>3904</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>3970</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>3867</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3905</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>3971</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>3867</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>3906</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0" t="s">
+        <v>3867</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3907</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>3973</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>3867</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3908</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>3868</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>3909</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>3868</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3910</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>3976</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>3868</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3911</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>3977</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>3912</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>3913</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>3979</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>3914</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B12" s="0"/>
+      <c r="C12" s="0"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>3870</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>3915</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>3981</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>3870</v>
+      </c>
+      <c r="B14" s="0"/>
+      <c r="C14" s="0"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>3870</v>
+      </c>
+      <c r="B15" s="0"/>
+      <c r="C15" s="0"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>3871</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>3916</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>3982</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>3871</v>
+      </c>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>3871</v>
+      </c>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>3872</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>3917</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>3983</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>3872</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>3918</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0" t="s">
+        <v>3873</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>3919</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>3985</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0" t="s">
+        <v>3873</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>3920</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>3873</v>
+      </c>
+      <c r="B23" s="0"/>
+      <c r="C23" s="0"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>3874</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>3921</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>3987</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>3874</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>3922</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>3988</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>3875</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>3923</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>3989</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>3876</v>
+      </c>
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>3877</v>
+      </c>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="0" t="s">
+        <v>3878</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>3924</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>3990</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="0" t="s">
+        <v>3879</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>3925</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>3991</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
+        <v>3880</v>
+      </c>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
+        <v>3881</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>3926</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>3882</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>3927</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>3993</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="s">
+        <v>3882</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>3928</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>3994</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="s">
+        <v>3882</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>3929</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>3995</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="s">
+        <v>3882</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>3930</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>3996</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="s">
+        <v>3883</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>3931</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="s">
+        <v>3883</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>3932</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>3998</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="s">
+        <v>3883</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>3933</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>3999</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="s">
+        <v>3884</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>3934</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="s">
+        <v>3884</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>3935</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>4001</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="s">
+        <v>3884</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>3936</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="s">
+        <v>3885</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>3937</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>4003</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="s">
+        <v>3886</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>3938</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>4004</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="s">
+        <v>3886</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>3939</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>4005</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="s">
+        <v>3887</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>3940</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="s">
+        <v>3888</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>3941</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="s">
+        <v>3889</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>3942</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>4008</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="s">
+        <v>3890</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>3943</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="s">
+        <v>3891</v>
+      </c>
+      <c r="B50" s="0" t="s">
+        <v>3944</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>4010</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="s">
+        <v>3892</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>3945</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="s">
+        <v>3893</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>3946</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>4012</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="s">
+        <v>3894</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>3947</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="s">
+        <v>3894</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>3948</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>4014</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="s">
+        <v>3894</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>3949</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="s">
+        <v>3895</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>3950</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>4016</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="s">
+        <v>3895</v>
+      </c>
+      <c r="B57" s="0" t="s">
+        <v>3951</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="s">
+        <v>3895</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>3952</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="s">
+        <v>3896</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>3953</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="s">
+        <v>3896</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>3954</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="s">
+        <v>3896</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>3955</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>4021</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="s">
+        <v>3896</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>3956</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="s">
+        <v>3896</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>3957</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>4023</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="s">
+        <v>3896</v>
+      </c>
+      <c r="B64" s="0" t="s">
+        <v>3958</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="s">
+        <v>3896</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>3959</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>4025</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="s">
+        <v>3896</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>3960</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>4026</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="s">
+        <v>3897</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>3961</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>4027</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="s">
+        <v>3898</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>3962</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>4028</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="s">
+        <v>3898</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>3963</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>4029</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="s">
+        <v>3899</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>3964</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>4030</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0" t="s">
+        <v>3900</v>
+      </c>
+      <c r="B71" s="0" t="s">
+        <v>3965</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="s">
+        <v>3901</v>
+      </c>
+      <c r="B72" s="0" t="s">
+        <v>3966</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>4032</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="0" t="s">
+        <v>3902</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>3967</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>4033</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="0" t="s">
+        <v>3902</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>3968</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>4034</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="0" t="s">
+        <v>3903</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>3969</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>4035</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>